<commit_message>
JH -- Length of code -- Calculate length of a particular code.
</commit_message>
<xml_diff>
--- a/Amanda.xlsx
+++ b/Amanda.xlsx
@@ -535,6 +535,11 @@
           <t>0:00:37,3</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0:00:24,200000</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="72" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -552,6 +557,11 @@
           <t>0:00:38,3</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="72" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
@@ -569,6 +579,11 @@
           <t>0:00:38,8</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="72" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -586,6 +601,11 @@
           <t>0:00:40,9</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0:00:00,200000</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="72" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
@@ -603,6 +623,11 @@
           <t>0:00:55,9</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0:00:01,500000</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="72" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -620,6 +645,11 @@
           <t>0:00:57,1</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="72" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -637,6 +667,11 @@
           <t>0:01:05,5</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0:00:08,200000</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="72" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -654,6 +689,11 @@
           <t>0:01:08,2</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="72" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
@@ -671,6 +711,11 @@
           <t>0:01:23,7</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0:00:15,400000</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="72" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
@@ -688,6 +733,11 @@
           <t>0:01:24,4</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="72" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
@@ -705,6 +755,11 @@
           <t>0:01:26,3</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="72" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
@@ -722,6 +777,11 @@
           <t>0:01:28,7</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="72" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
@@ -739,6 +799,11 @@
           <t>0:01:32,0</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="72" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
@@ -756,6 +821,11 @@
           <t>0:01:55,5</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0:00:06,900000</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="72" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
@@ -773,6 +843,11 @@
           <t>0:01:56,2</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="72" customHeight="1">
       <c r="A18" s="2" t="inlineStr">
@@ -790,6 +865,11 @@
           <t>0:02:05,7</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0:00:08,900000</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="72" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
@@ -807,6 +887,11 @@
           <t>0:02:06,0</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="72" customHeight="1">
       <c r="A20" s="2" t="inlineStr">
@@ -824,6 +909,11 @@
           <t>0:02:16,1</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0:00:10</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="72" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
@@ -841,6 +931,11 @@
           <t>0:02:16,8</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="72" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
@@ -858,6 +953,11 @@
           <t>0:02:19,1</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="72" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
@@ -875,6 +975,11 @@
           <t>0:02:19,5</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="72" customHeight="1">
       <c r="A24" s="2" t="inlineStr">
@@ -892,6 +997,11 @@
           <t>0:02:34,9</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0:00:15,100000</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="72" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
@@ -909,6 +1019,11 @@
           <t>0:02:36,2</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="72" customHeight="1">
       <c r="A26" s="2" t="inlineStr">
@@ -926,6 +1041,11 @@
           <t>0:02:40,4</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0:00:04,100000</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="72" customHeight="1">
       <c r="A27" s="2" t="inlineStr">
@@ -943,6 +1063,11 @@
           <t>0:02:40,8</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="72" customHeight="1">
       <c r="A28" s="2" t="inlineStr">
@@ -960,6 +1085,11 @@
           <t>0:02:45,7</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0:00:04,500000</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="72" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
@@ -977,6 +1107,11 @@
           <t>0:02:59,0</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0:00:12,700000</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="72" customHeight="1">
       <c r="A30" s="2" t="inlineStr">
@@ -994,6 +1129,11 @@
           <t>0:02:59,6</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="72" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
@@ -1011,6 +1151,11 @@
           <t>0:03:01,2</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="72" customHeight="1">
       <c r="A32" s="2" t="inlineStr">
@@ -1028,6 +1173,11 @@
           <t>0:03:03,5</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="72" customHeight="1">
       <c r="A33" s="2" t="inlineStr">
@@ -1045,6 +1195,11 @@
           <t>0:03:06,7</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="72" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
@@ -1062,6 +1217,11 @@
           <t>0:03:08,3</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="72" customHeight="1">
       <c r="A35" s="2" t="inlineStr">
@@ -1079,6 +1239,11 @@
           <t>0:03:13,0</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0:00:04,200000</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="72" customHeight="1">
       <c r="A36" s="2" t="inlineStr">
@@ -1096,6 +1261,11 @@
           <t>0:03:13,5</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="72" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
@@ -1113,6 +1283,11 @@
           <t>0:03:30,9</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0:00:06,400000</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="72" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
@@ -1130,6 +1305,11 @@
           <t>0:03:32,8</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="72" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
@@ -1147,6 +1327,11 @@
           <t>0:03:38,7</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0:00:05,500000</t>
+        </is>
+      </c>
     </row>
     <row r="40" ht="72" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
@@ -1164,6 +1349,11 @@
           <t>0:03:39,4</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="72" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
@@ -1181,6 +1371,11 @@
           <t>0:03:51,6</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
     </row>
     <row r="42" ht="72" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
@@ -1198,6 +1393,11 @@
           <t>0:03:52,0</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="43" ht="72" customHeight="1">
       <c r="A43" s="2" t="inlineStr">
@@ -1215,6 +1415,11 @@
           <t>0:03:52,9</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="44" ht="72" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
@@ -1232,6 +1437,11 @@
           <t>0:03:56,6</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0:00:02,500000</t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="72" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
@@ -1249,6 +1459,11 @@
           <t>0:04:05,8</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="46" ht="72" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
@@ -1266,6 +1481,11 @@
           <t>0:04:07,0</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="47" ht="72" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
@@ -1283,6 +1503,11 @@
           <t>0:04:07,5</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="72" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
@@ -1300,6 +1525,11 @@
           <t>0:04:08,9</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0:00:01,300000</t>
+        </is>
+      </c>
     </row>
     <row r="49" ht="72" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
@@ -1317,6 +1547,11 @@
           <t>0:04:09,1</t>
         </is>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0:00:00,100000</t>
+        </is>
+      </c>
     </row>
     <row r="50" ht="72" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
@@ -1334,6 +1569,11 @@
           <t>0:04:21,6</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0:00:12,400000</t>
+        </is>
+      </c>
     </row>
     <row r="51" ht="72" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
@@ -1351,6 +1591,11 @@
           <t>0:04:22,2</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="52" ht="72" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
@@ -1368,6 +1613,11 @@
           <t>0:04:44,0</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="53" ht="72" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
@@ -1385,6 +1635,11 @@
           <t>0:04:46,0</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0:00:01,700000</t>
+        </is>
+      </c>
     </row>
     <row r="54" ht="72" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
@@ -1402,6 +1657,11 @@
           <t>0:04:47,3</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="55" ht="72" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
@@ -1419,6 +1679,11 @@
           <t>0:04:48,2</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="72" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
@@ -1436,6 +1701,11 @@
           <t>0:04:54,1</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0:00:05,200000</t>
+        </is>
+      </c>
     </row>
     <row r="57" ht="72" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
@@ -1453,6 +1723,11 @@
           <t>0:04:54,4</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="58" ht="72" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
@@ -1470,6 +1745,11 @@
           <t>0:05:02,6</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0:00:07,200000</t>
+        </is>
+      </c>
     </row>
     <row r="59" ht="72" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
@@ -1487,6 +1767,11 @@
           <t>0:05:03,8</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
     <row r="60" ht="72" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
@@ -1504,6 +1789,11 @@
           <t>0:05:19,2</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0:00:04,800000</t>
+        </is>
+      </c>
     </row>
     <row r="61" ht="72" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
@@ -1521,6 +1811,11 @@
           <t>0:05:20,8</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="62" ht="72" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
@@ -1538,6 +1833,11 @@
           <t>0:05:28,4</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0:00:06,900000</t>
+        </is>
+      </c>
     </row>
     <row r="63" ht="72" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
@@ -1555,6 +1855,11 @@
           <t>0:05:29,6</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0:00:01,200000</t>
+        </is>
+      </c>
     </row>
     <row r="64" ht="72" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
@@ -1572,6 +1877,11 @@
           <t>0:05:30,0</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="65" ht="72" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
@@ -1589,6 +1899,11 @@
           <t>0:05:31,6</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0:00:01,400000</t>
+        </is>
+      </c>
     </row>
     <row r="66" ht="72" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
@@ -1606,6 +1921,11 @@
           <t>0:06:08,7</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0:00:06,700000</t>
+        </is>
+      </c>
     </row>
     <row r="67" ht="72" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
@@ -1623,6 +1943,11 @@
           <t>0:06:09,5</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="68" ht="72" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
@@ -1640,6 +1965,11 @@
           <t>0:06:10,0</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="69" ht="72" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
@@ -1657,6 +1987,11 @@
           <t>0:06:10,6</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="70" ht="72" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
@@ -1674,6 +2009,11 @@
           <t>0:06:12,1</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0:00:01,300000</t>
+        </is>
+      </c>
     </row>
     <row r="71" ht="72" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
@@ -1691,6 +2031,11 @@
           <t>0:06:12,6</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="72" ht="72" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
@@ -1708,6 +2053,11 @@
           <t>0:06:47,4</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0:00:02,700000</t>
+        </is>
+      </c>
     </row>
     <row r="73" ht="72" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
@@ -1725,6 +2075,11 @@
           <t>0:06:47,6</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0:00:00,200000</t>
+        </is>
+      </c>
     </row>
     <row r="74" ht="72" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
@@ -1742,6 +2097,11 @@
           <t>0:06:48,2</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="75" ht="72" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
@@ -1759,6 +2119,11 @@
           <t>0:06:52,9</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
     </row>
     <row r="76" ht="72" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
@@ -1776,6 +2141,11 @@
           <t>0:06:54,3</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0:00:01,400000</t>
+        </is>
+      </c>
     </row>
     <row r="77" ht="72" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
@@ -1793,6 +2163,11 @@
           <t>0:07:02,7</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0:00:06,700000</t>
+        </is>
+      </c>
     </row>
     <row r="78" ht="72" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
@@ -1810,6 +2185,11 @@
           <t>0:07:03,0</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="79" ht="72" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
@@ -1827,6 +2207,11 @@
           <t>0:08:03,0</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0:00:11,600000</t>
+        </is>
+      </c>
     </row>
     <row r="80" ht="72" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
@@ -1844,6 +2229,11 @@
           <t>0:08:03,8</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="81" ht="72" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
@@ -1861,6 +2251,11 @@
           <t>0:08:11,2</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0:00:07,300000</t>
+        </is>
+      </c>
     </row>
     <row r="82" ht="72" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
@@ -1878,6 +2273,11 @@
           <t>0:08:14,9</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0:00:03,600000</t>
+        </is>
+      </c>
     </row>
     <row r="83" ht="72" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
@@ -1895,6 +2295,11 @@
           <t>0:08:33,5</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
     </row>
     <row r="84" ht="72" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
@@ -1912,6 +2317,11 @@
           <t>0:08:33,9</t>
         </is>
       </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="85" ht="72" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
@@ -1929,6 +2339,11 @@
           <t>0:08:36,0</t>
         </is>
       </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0:00:01,900000</t>
+        </is>
+      </c>
     </row>
     <row r="86" ht="72" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
@@ -1946,6 +2361,11 @@
           <t>0:08:36,4</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="72" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
@@ -1963,6 +2383,11 @@
           <t>0:08:37,6</t>
         </is>
       </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0:00:01,100000</t>
+        </is>
+      </c>
     </row>
     <row r="88" ht="72" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
@@ -1980,6 +2405,11 @@
           <t>0:08:38,8</t>
         </is>
       </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="89" ht="72" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
@@ -1997,6 +2427,11 @@
           <t>0:08:40,5</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0:00:01,500000</t>
+        </is>
+      </c>
     </row>
     <row r="90" ht="72" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
@@ -2014,6 +2449,11 @@
           <t>0:08:49,2</t>
         </is>
       </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0:00:08,400000</t>
+        </is>
+      </c>
     </row>
     <row r="91" ht="72" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
@@ -2031,6 +2471,11 @@
           <t>0:08:49,6</t>
         </is>
       </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="92" ht="72" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
@@ -2048,6 +2493,11 @@
           <t>0:08:50,1</t>
         </is>
       </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="93" ht="72" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
@@ -2065,6 +2515,11 @@
           <t>0:08:50,7</t>
         </is>
       </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="94" ht="72" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
@@ -2082,6 +2537,11 @@
           <t>0:08:52,7</t>
         </is>
       </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
     </row>
     <row r="95" ht="72" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
@@ -2099,6 +2559,11 @@
           <t>0:09:10,6</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0:00:03,200000</t>
+        </is>
+      </c>
     </row>
     <row r="96" ht="72" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
@@ -2116,6 +2581,11 @@
           <t>0:09:11,3</t>
         </is>
       </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="97" ht="72" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
@@ -2133,6 +2603,11 @@
           <t>0:09:12,6</t>
         </is>
       </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="98" ht="72" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
@@ -2150,6 +2625,11 @@
           <t>0:09:13,5</t>
         </is>
       </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="99" ht="72" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
@@ -2167,6 +2647,11 @@
           <t>0:09:19,9</t>
         </is>
       </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0:00:06,400000</t>
+        </is>
+      </c>
     </row>
     <row r="100" ht="72" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
@@ -2184,6 +2669,11 @@
           <t>0:09:20,4</t>
         </is>
       </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="101" ht="72" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
@@ -2201,6 +2691,11 @@
           <t>0:09:21,4</t>
         </is>
       </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0:00:00,300000</t>
+        </is>
+      </c>
     </row>
     <row r="102" ht="72" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
@@ -2218,6 +2713,11 @@
           <t>0:09:22,8</t>
         </is>
       </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>0:00:01,500000</t>
+        </is>
+      </c>
     </row>
     <row r="103" ht="72" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
@@ -2235,6 +2735,11 @@
           <t>0:09:23,4</t>
         </is>
       </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0:00:00,500000</t>
+        </is>
+      </c>
     </row>
     <row r="104" ht="72" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
@@ -2252,6 +2757,11 @@
           <t>0:09:25,7</t>
         </is>
       </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>0:00:01,700000</t>
+        </is>
+      </c>
     </row>
     <row r="105" ht="72" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
@@ -2269,6 +2779,11 @@
           <t>0:10:00,0</t>
         </is>
       </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="106" ht="72" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
@@ -2286,6 +2801,11 @@
           <t>0:10:00,7</t>
         </is>
       </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0:00:00,700000</t>
+        </is>
+      </c>
     </row>
     <row r="107" ht="72" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
@@ -2303,6 +2823,11 @@
           <t>0:10:01,6</t>
         </is>
       </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="108" ht="72" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
@@ -2320,6 +2845,11 @@
           <t>0:10:02,3</t>
         </is>
       </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0:00:00,600000</t>
+        </is>
+      </c>
     </row>
     <row r="109" ht="72" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
@@ -2337,6 +2867,11 @@
           <t>0:10:07,3</t>
         </is>
       </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0:00:04,900000</t>
+        </is>
+      </c>
     </row>
     <row r="110" ht="72" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
@@ -2354,6 +2889,11 @@
           <t>0:10:08,4</t>
         </is>
       </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
     <row r="111" ht="72" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
@@ -2371,6 +2911,11 @@
           <t>0:10:09,4</t>
         </is>
       </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
     <row r="112" ht="72" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
@@ -2388,6 +2933,11 @@
           <t>0:10:14,7</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>0:00:05,200000</t>
+        </is>
+      </c>
     </row>
     <row r="113" ht="72" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
@@ -2405,6 +2955,11 @@
           <t>0:10:27,2</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>0:00:00,900000</t>
+        </is>
+      </c>
     </row>
     <row r="114" ht="72" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
@@ -2422,6 +2977,11 @@
           <t>0:10:27,6</t>
         </is>
       </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>0:00:00,400000</t>
+        </is>
+      </c>
     </row>
     <row r="115" ht="72" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
@@ -2437,6 +2997,11 @@
       <c r="C115" s="2" t="inlineStr">
         <is>
           <t>0:10:32,3</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>0:00:04,600000</t>
         </is>
       </c>
     </row>

</xml_diff>